<commit_message>
Merged data of 2015 batch
</commit_message>
<xml_diff>
--- a/Cleaned-Data/2015-Passouts/2015_merged.xlsx
+++ b/Cleaned-Data/2015-Passouts/2015_merged.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prashant/Downloads/Student-Placement-Guidance/Cleaned-Data/2015-Passouts/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16040"/>
   </bookViews>
   <sheets>
     <sheet name="2015_merged" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -538,8 +551,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,6 +615,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -648,12 +666,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -680,14 +698,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -714,6 +733,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -889,14 +909,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="11" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="4" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="9" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="10" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:85">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
@@ -1153,7 +1258,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:85">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1407,7 +1512,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:85">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>82</v>
       </c>
@@ -1664,7 +1769,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:85">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>83</v>
       </c>
@@ -1921,7 +2026,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:85">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
@@ -2178,7 +2283,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:85">
+    <row r="6" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>85</v>
       </c>
@@ -2432,7 +2537,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:85">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>86</v>
       </c>
@@ -2686,7 +2791,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:85">
+    <row r="8" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -2943,7 +3048,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:85">
+    <row r="9" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>88</v>
       </c>
@@ -3188,7 +3293,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:85">
+    <row r="10" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
@@ -3442,7 +3547,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:85">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>90</v>
       </c>
@@ -3696,7 +3801,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:85">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>91</v>
       </c>
@@ -3953,7 +4058,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:85">
+    <row r="13" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>92</v>
       </c>
@@ -4207,7 +4312,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:85">
+    <row r="14" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>93</v>
       </c>
@@ -4461,7 +4566,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:85">
+    <row r="15" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>94</v>
       </c>
@@ -4715,7 +4820,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:85">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>95</v>
       </c>
@@ -4969,7 +5074,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:85">
+    <row r="17" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>96</v>
       </c>
@@ -5223,7 +5328,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:85">
+    <row r="18" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>97</v>
       </c>
@@ -5480,7 +5585,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:85">
+    <row r="19" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>98</v>
       </c>
@@ -5734,7 +5839,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:85">
+    <row r="20" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>99</v>
       </c>
@@ -5988,7 +6093,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:85">
+    <row r="21" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>100</v>
       </c>
@@ -6242,7 +6347,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:85">
+    <row r="22" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>101</v>
       </c>
@@ -6481,7 +6586,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:85">
+    <row r="23" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>102</v>
       </c>
@@ -6735,7 +6840,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:85">
+    <row r="24" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>103</v>
       </c>
@@ -6989,7 +7094,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="1:85">
+    <row r="25" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>104</v>
       </c>
@@ -7243,7 +7348,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:85">
+    <row r="26" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>105</v>
       </c>
@@ -7497,7 +7602,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:85">
+    <row r="27" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>106</v>
       </c>
@@ -7751,7 +7856,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:85">
+    <row r="28" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>107</v>
       </c>
@@ -8005,7 +8110,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:85">
+    <row r="29" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>108</v>
       </c>
@@ -8259,7 +8364,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:85">
+    <row r="30" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>109</v>
       </c>
@@ -8513,7 +8618,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:85">
+    <row r="31" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>110</v>
       </c>
@@ -8767,7 +8872,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:85">
+    <row r="32" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>111</v>
       </c>
@@ -9021,7 +9126,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:85">
+    <row r="33" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>112</v>
       </c>
@@ -9275,7 +9380,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="34" spans="1:85">
+    <row r="34" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>113</v>
       </c>
@@ -9520,7 +9625,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="1:85">
+    <row r="35" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>114</v>
       </c>
@@ -9774,7 +9879,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:85">
+    <row r="36" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>115</v>
       </c>
@@ -10031,7 +10136,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:85">
+    <row r="37" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>116</v>
       </c>
@@ -10285,7 +10390,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="38" spans="1:85">
+    <row r="38" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>117</v>
       </c>
@@ -10539,7 +10644,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:85">
+    <row r="39" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>118</v>
       </c>
@@ -10793,7 +10898,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:85">
+    <row r="40" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>119</v>
       </c>
@@ -11047,7 +11152,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:85">
+    <row r="41" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>120</v>
       </c>
@@ -11295,7 +11400,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:85">
+    <row r="42" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>121</v>
       </c>
@@ -11552,7 +11657,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:85">
+    <row r="43" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>122</v>
       </c>
@@ -11806,7 +11911,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:85">
+    <row r="44" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>123</v>
       </c>
@@ -12060,7 +12165,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="45" spans="1:85">
+    <row r="45" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>124</v>
       </c>
@@ -12311,7 +12416,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:85">
+    <row r="46" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>125</v>
       </c>
@@ -12559,7 +12664,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:85">
+    <row r="47" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>126</v>
       </c>
@@ -12816,7 +12921,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:85">
+    <row r="48" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>127</v>
       </c>
@@ -13073,7 +13178,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:85">
+    <row r="49" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>128</v>
       </c>
@@ -13327,7 +13432,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="1:85">
+    <row r="50" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>129</v>
       </c>
@@ -13581,7 +13686,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:85">
+    <row r="51" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>130</v>
       </c>
@@ -13835,7 +13940,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:85">
+    <row r="52" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>131</v>
       </c>
@@ -14092,7 +14197,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:85">
+    <row r="53" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>132</v>
       </c>
@@ -14346,7 +14451,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:85">
+    <row r="54" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>133</v>
       </c>
@@ -14600,7 +14705,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:85">
+    <row r="55" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>134</v>
       </c>
@@ -14854,7 +14959,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:85">
+    <row r="56" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>135</v>
       </c>
@@ -15108,7 +15213,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="57" spans="1:85">
+    <row r="57" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>136</v>
       </c>
@@ -15359,7 +15464,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="58" spans="1:85">
+    <row r="58" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>137</v>
       </c>
@@ -15613,7 +15718,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="1:85">
+    <row r="59" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>138</v>
       </c>
@@ -15867,7 +15972,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="60" spans="1:85">
+    <row r="60" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>139</v>
       </c>
@@ -16121,7 +16226,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="1:85">
+    <row r="61" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>140</v>
       </c>
@@ -16378,7 +16483,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="62" spans="1:85">
+    <row r="62" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>141</v>
       </c>
@@ -16632,7 +16737,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="1:85">
+    <row r="63" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>142</v>
       </c>
@@ -16886,7 +16991,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:85">
+    <row r="64" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>143</v>
       </c>
@@ -17140,7 +17245,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:85">
+    <row r="65" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>144</v>
       </c>
@@ -17394,7 +17499,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:85">
+    <row r="66" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>145</v>
       </c>
@@ -17651,7 +17756,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="67" spans="1:85">
+    <row r="67" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>146</v>
       </c>
@@ -17905,7 +18010,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:85">
+    <row r="68" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>147</v>
       </c>
@@ -18162,7 +18267,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:85">
+    <row r="69" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>148</v>
       </c>
@@ -18419,7 +18524,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="70" spans="1:85">
+    <row r="70" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>149</v>
       </c>
@@ -18676,7 +18781,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="71" spans="1:85">
+    <row r="71" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>150</v>
       </c>
@@ -18927,7 +19032,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="72" spans="1:85">
+    <row r="72" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>151</v>
       </c>
@@ -19184,7 +19289,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="73" spans="1:85">
+    <row r="73" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>152</v>
       </c>
@@ -19438,7 +19543,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:85">
+    <row r="74" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>153</v>
       </c>
@@ -19692,7 +19797,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="75" spans="1:85">
+    <row r="75" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>154</v>
       </c>

</xml_diff>